<commit_message>
Added examples of DataFormat, autoSizing columns and merging cells.
</commit_message>
<xml_diff>
--- a/GUS_JAVA/createworkbook.xlsx
+++ b/GUS_JAVA/createworkbook.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Your Report" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Your Report'!$A$1:$C$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Your Report'!$A$1:$C$5</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -26,7 +26,8 @@
     <t>Utilization%</t>
   </si>
   <si>
-    <t>Manager, Mike</t>
+    <t>Manager, Mike 
+(PMP)</t>
   </si>
   <si>
     <t>Manager</t>
@@ -48,7 +49,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11.0"/>
@@ -101,10 +104,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -117,6 +126,11 @@
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.53515625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.93359375" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
@@ -129,45 +143,48 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" ht="30.0" customHeight="true">
+      <c r="A2" t="s" s="3">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>76.0</v>
+      <c r="C2" t="n" s="2">
+        <v>0.76</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="3" ht="30.0" customHeight="true">
+      <c r="A3" t="s" s="3">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>95.0</v>
+      <c r="C3" t="n" s="2">
+        <v>0.95</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="4" ht="30.0" customHeight="true">
+      <c r="A4" t="s" s="3">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>90.0</v>
+      <c r="C4" t="n" s="2">
+        <v>0.88</v>
       </c>
     </row>
     <row r="5">
-      <c r="C5">
+      <c r="A5">
         <f>SUM(C2:C4)</f>
       </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
   <printOptions gridLines="true"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9"/>

</xml_diff>